<commit_message>
integrated s3 to reports and inventory
</commit_message>
<xml_diff>
--- a/docs/invoice12.xlsx
+++ b/docs/invoice12.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Invoice Template" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Invoice Template" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -2121,7 +2121,7 @@
       <c r="A5" s="7" t="n"/>
       <c r="B5" s="52" t="inlineStr">
         <is>
-          <t>02/29/2024</t>
+          <t>03/12/2024</t>
         </is>
       </c>
       <c r="D5" s="88" t="n"/>
@@ -2134,7 +2134,7 @@
       <c r="K5" s="83" t="n"/>
       <c r="L5" s="96" t="inlineStr">
         <is>
-          <t>QR02292024AP101</t>
+          <t>QR03122024AP01</t>
         </is>
       </c>
       <c r="M5" s="97" t="n"/>
@@ -2194,7 +2194,7 @@
       <c r="A10" s="36" t="n"/>
       <c r="B10" s="78" t="inlineStr">
         <is>
-          <t>AUTREY PHARMACY 1</t>
+          <t>Alamo Pharmacy IPBG</t>
         </is>
       </c>
       <c r="D10" s="58" t="inlineStr">
@@ -2204,7 +2204,7 @@
       </c>
       <c r="E10" s="77" t="inlineStr">
         <is>
-          <t>AUTREY PHARMACY 1</t>
+          <t>Alamo Pharmacy IPBG</t>
         </is>
       </c>
       <c r="H10" s="99" t="n"/>
@@ -2216,7 +2216,7 @@
       <c r="A11" s="36" t="n"/>
       <c r="B11" s="78" t="inlineStr">
         <is>
-          <t>1205 CENTRAL BLVD</t>
+          <t>BROWNSVILLE TX 78521-3212</t>
         </is>
       </c>
       <c r="D11" s="58" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="E11" s="77" t="inlineStr">
         <is>
-          <t>1205 CENTRAL BLVD</t>
+          <t>BROWNSVILLE TX 78521-3212</t>
         </is>
       </c>
       <c r="H11" s="82" t="n"/>
@@ -2236,21 +2236,13 @@
     </row>
     <row r="12" ht="18" customHeight="1" s="76">
       <c r="A12" s="36" t="n"/>
-      <c r="B12" s="78" t="inlineStr">
-        <is>
-          <t>BROWNSVILLE, TX, 78520</t>
-        </is>
-      </c>
+      <c r="B12" s="78" t="inlineStr"/>
       <c r="D12" s="58" t="inlineStr">
         <is>
           <t>WHITESTONE, NY,11357</t>
         </is>
       </c>
-      <c r="E12" s="77" t="inlineStr">
-        <is>
-          <t>BROWNSVILLE, TX, 78520</t>
-        </is>
-      </c>
+      <c r="E12" s="77" t="inlineStr"/>
       <c r="H12" s="82" t="n"/>
       <c r="L12" s="12" t="n"/>
       <c r="M12" s="12" t="n"/>
@@ -2282,7 +2274,7 @@
       <c r="A14" s="36" t="n"/>
       <c r="B14" s="78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Phone: 956-548-0801, fax: </t>
+          <t xml:space="preserve">Phone: , fax: </t>
         </is>
       </c>
       <c r="D14" s="77" t="inlineStr">
@@ -2292,7 +2284,7 @@
       </c>
       <c r="E14" s="77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Phone: 956-548-0801, fax: </t>
+          <t xml:space="preserve">Phone: , fax: </t>
         </is>
       </c>
       <c r="H14" s="75" t="n"/>
@@ -2304,7 +2296,7 @@
       <c r="A15" s="36" t="n"/>
       <c r="B15" s="78" t="inlineStr">
         <is>
-          <t>DEA: FA3704358, Exp: 06/30/2023</t>
+          <t>DEA: FU7640661, Exp: 06/30/2024</t>
         </is>
       </c>
       <c r="D15" s="77" t="inlineStr">
@@ -2314,7 +2306,7 @@
       </c>
       <c r="E15" s="77" t="inlineStr">
         <is>
-          <t>DEA: FA3704358, Exp: 06/30/2023</t>
+          <t>DEA: FU7640661, Exp: 06/30/2024</t>
         </is>
       </c>
       <c r="H15" s="75" t="n"/>
@@ -2326,13 +2318,13 @@
       <c r="A16" s="36" t="n"/>
       <c r="B16" s="78" t="inlineStr">
         <is>
-          <t>Authorized Classes: 2, 2N, 3, 3N, 4. 5</t>
+          <t xml:space="preserve">Authorized Classes: </t>
         </is>
       </c>
       <c r="D16" s="77" t="n"/>
       <c r="E16" s="77" t="inlineStr">
         <is>
-          <t>Authorized Classes: 2, 2N, 3, 3N, 4. 5</t>
+          <t xml:space="preserve">Authorized Classes: </t>
         </is>
       </c>
       <c r="H16" s="75" t="n"/>
@@ -2430,57 +2422,53 @@
       <c r="A20" s="37" t="n"/>
       <c r="B20" s="28" t="inlineStr">
         <is>
-          <t>47335037983</t>
+          <t>6787743305</t>
         </is>
       </c>
       <c r="C20" s="29" t="inlineStr">
         <is>
-          <t>Sun Pharmaceutical Industries, Inc.</t>
+          <t>Ascend Laboratories, LLC</t>
         </is>
       </c>
       <c r="D20" s="29" t="inlineStr">
         <is>
-          <t>Cinacalcet</t>
+          <t>Aripiprazole</t>
         </is>
       </c>
       <c r="E20" s="30" t="inlineStr">
         <is>
-          <t>30 mg/1</t>
+          <t>15 mg/1</t>
         </is>
       </c>
       <c r="F20" s="30" t="inlineStr">
         <is>
-          <t>TABLET, FILM COATED</t>
+          <t>TABLET</t>
         </is>
       </c>
       <c r="G20" s="30" t="inlineStr">
         <is>
-          <t>DND0467A</t>
+          <t>22140477</t>
         </is>
       </c>
       <c r="H20" s="30" t="inlineStr">
         <is>
-          <t>02/24</t>
+          <t>01/24/31</t>
         </is>
       </c>
       <c r="I20" s="30" t="inlineStr">
         <is>
-          <t>30 CT</t>
-        </is>
-      </c>
-      <c r="J20" s="30" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+          <t>500 CT</t>
+        </is>
+      </c>
+      <c r="J20" s="30" t="n">
+        <v>1</v>
       </c>
       <c r="K20" s="30" t="n"/>
-      <c r="L20" s="30" t="inlineStr">
-        <is>
-          <t>280</t>
-        </is>
+      <c r="L20" s="30" t="n">
+        <v>1</v>
       </c>
       <c r="M20" s="30" t="n">
-        <v>6720</v>
+        <v>1</v>
       </c>
       <c r="N20" s="19" t="n"/>
     </row>
@@ -3241,7 +3229,7 @@
       <c r="K66" s="33" t="n"/>
       <c r="L66" s="33" t="n"/>
       <c r="M66" s="33" t="n">
-        <v>6720</v>
+        <v>1</v>
       </c>
       <c r="N66" s="69" t="n"/>
       <c r="O66" s="84" t="n"/>

</xml_diff>